<commit_message>
closing 2 reviews 1-Rv_28 2-Rv_29
</commit_message>
<xml_diff>
--- a/Managment/Plans/ACS_RL.xlsx
+++ b/Managment/Plans/ACS_RL.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
   <si>
     <t>Air Conditioner Screen Review Log</t>
   </si>
@@ -378,9 +378,6 @@
     <t>04/15/2018</t>
   </si>
   <si>
-    <t>ACS_SRS V1.1</t>
-  </si>
-  <si>
     <t>Hadeel Yamni</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
   </si>
   <si>
     <t>in relevant data is written in introduction section, i.e remove what is written in section introduction 1</t>
-  </si>
-  <si>
-    <t>ACS_SRS V1.3</t>
   </si>
   <si>
     <t>update the version of the SRS</t>
@@ -473,12 +467,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -503,12 +491,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -796,7 +790,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -811,787 +805,787 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>43104</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>43194</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>43194</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>43194</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>43194</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>43194</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>43224</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <v>43255</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <v>43255</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="13.5" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:7" s="15" customFormat="1" ht="13.5" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="8" t="s">
+      <c r="D21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="8" t="s">
+      <c r="D22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="54" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="27" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="9">
         <v>43408</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:7" s="12" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="15" t="s">
+    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="12" t="s">
+      <c r="F31" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="G31" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="D32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="10" t="s">
+    <row r="33" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G33" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="12" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="12" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="12" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="12" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="12" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="12" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="12" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="12" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="12" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1629,12 +1623,12 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Closing opened reviews about the test plan.
</commit_message>
<xml_diff>
--- a/Managment/Plans/ACS_RL.xlsx
+++ b/Managment/Plans/ACS_RL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Air-Conditioner-Screen-Team-4\Managment\Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\iTi - QA &amp; Testing (intake 38)\Project Management Project\Air-Conditioner-Screen-Team-4\Managment\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16812" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -789,19 +789,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1"/>
-    <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="1"/>
+    <col min="2" max="2" width="36.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="1"/>
+    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -838,7 +838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -861,7 +861,7 @@
         <v>43104</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -884,7 +884,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -907,7 +907,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -930,7 +930,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -953,7 +953,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -976,7 +976,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
@@ -999,7 +999,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
@@ -1045,8 +1045,8 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="15" customFormat="1" ht="13.5" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="15" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>73</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>34</v>
@@ -1277,7 +1277,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>34</v>
@@ -1307,7 +1307,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>34</v>
@@ -1361,7 +1361,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>84</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>85</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1620,14 +1620,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
CDD_LCD commented with missed parts
</commit_message>
<xml_diff>
--- a/Managment/Plans/ACS_RL.xlsx
+++ b/Managment/Plans/ACS_RL.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismail samy\Desktop\GIT\Managment\Plans\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B2E561DC-59C3-44EE-9E48-1D9AEA1AD0D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16812" windowHeight="7752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
   <si>
     <t>Air Conditioner Screen Review Log</t>
   </si>
@@ -403,12 +409,24 @@
   <si>
     <t>update the version of the CDD_Timer</t>
   </si>
+  <si>
+    <t xml:space="preserve">sequence diagram not found, mode management block diagram </t>
+  </si>
+  <si>
+    <t>CDD_LCD</t>
+  </si>
+  <si>
+    <t>ismail samy</t>
+  </si>
+  <si>
+    <t>update the version of the CDD_LCD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -436,6 +454,12 @@
       <sz val="10"/>
       <color theme="4"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -471,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,6 +544,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,29 +818,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1"/>
-    <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="1"/>
+    <col min="2" max="2" width="36.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="1"/>
+    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -828,7 +854,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -851,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -874,7 +900,7 @@
         <v>43104</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -897,7 +923,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -920,7 +946,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -943,7 +969,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -966,7 +992,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -989,7 +1015,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
@@ -1012,7 +1038,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
@@ -1035,7 +1061,7 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
@@ -1058,8 +1084,8 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="13.5" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -1080,7 +1106,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -1164,7 +1190,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -1185,7 +1211,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
@@ -1206,7 +1232,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
@@ -1227,7 +1253,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -1269,7 +1295,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>73</v>
       </c>
@@ -1290,7 +1316,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
@@ -1374,7 +1400,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>84</v>
       </c>
@@ -1395,7 +1421,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>85</v>
       </c>
@@ -1417,7 +1443,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1504,16 +1530,36 @@
       <c r="A35" s="12" t="s">
         <v>90</v>
       </c>
+      <c r="B35" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="19">
+        <v>43210</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>91</v>
       </c>
+      <c r="B36"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>92</v>
       </c>
+      <c r="B37"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
@@ -1631,7 +1677,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$2</xm:f>
           </x14:formula1>
@@ -1644,21 +1690,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added the CDD_timer Review
</commit_message>
<xml_diff>
--- a/Managment/Plans/ACS_RL.xlsx
+++ b/Managment/Plans/ACS_RL.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\iTi - QA &amp; Testing (intake 38)\Project Management Project\Air-Conditioner-Screen-Team-4\Managment\Plans\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16812" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
   <si>
     <t>Air Conditioner Screen Review Log</t>
   </si>
@@ -392,6 +387,21 @@
   </si>
   <si>
     <t>update the version of the SRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History Section is empty without date creation </t>
+  </si>
+  <si>
+    <t>CCD_TIMER</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Youssef Medhat</t>
+  </si>
+  <si>
+    <t>update the version of the CDD_Timer</t>
   </si>
 </sst>
 </file>
@@ -461,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -493,6 +503,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,7 +580,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,7 +615,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,7 +792,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -789,33 +802,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1"/>
-    <col min="2" max="2" width="36.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1"/>
+    <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.44140625" style="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -838,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -861,7 +874,7 @@
         <v>43104</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -884,7 +897,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -907,7 +920,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -930,7 +943,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -953,7 +966,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -976,7 +989,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
@@ -999,7 +1012,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
@@ -1022,7 +1035,7 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
@@ -1045,8 +1058,8 @@
         <v>43255</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="15" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="13.5" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -1067,7 +1080,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -1151,7 +1164,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -1172,7 +1185,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
@@ -1193,7 +1206,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
@@ -1214,7 +1227,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -1256,7 +1269,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>73</v>
       </c>
@@ -1277,7 +1290,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
@@ -1361,7 +1374,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>84</v>
       </c>
@@ -1382,7 +1395,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>85</v>
       </c>
@@ -1403,8 +1416,8 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1464,9 +1477,27 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>89</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="9">
+        <v>43210</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,14 +1651,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
adding 3 reviews about HLD 1-HLD document version is out of date 2-secion 4in HLD is missing 3-section 5 in HLD is missing
</commit_message>
<xml_diff>
--- a/Managment/Plans/ACS_RL.xlsx
+++ b/Managment/Plans/ACS_RL.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismail samy\Desktop\GIT\Managment\Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Air-Conditioner-Screen-Team-4\Managment\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B2E561DC-59C3-44EE-9E48-1D9AEA1AD0D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16812" windowHeight="7752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="145">
   <si>
     <t>Air Conditioner Screen Review Log</t>
   </si>
@@ -421,23 +420,66 @@
   <si>
     <t>update the version of the CDD_LCD</t>
   </si>
+  <si>
+    <t>tabel of content isnot updated in SRS</t>
+  </si>
+  <si>
+    <t>In relevant data written in introduction section
+in srs</t>
+  </si>
+  <si>
+    <t>version of srs is out of date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File is corrupted and doesnot open </t>
+  </si>
+  <si>
+    <t>section 4 System Features is un complete
+ (missing completely)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLD </t>
+  </si>
+  <si>
+    <t>section 5 High Level Design Decision is un complete (missing completely)</t>
+  </si>
+  <si>
+    <t>HLD version is missing</t>
+  </si>
+  <si>
+    <t>04/19/2018</t>
+  </si>
+  <si>
+    <t>04/20/2018</t>
+  </si>
+  <si>
+    <t>HLD file dosenot open</t>
+  </si>
+  <si>
+    <t>section 4 in HLD is missing</t>
+  </si>
+  <si>
+    <t>section 5 in HLD is missing</t>
+  </si>
+  <si>
+    <t>version of HLD is out of date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -457,13 +499,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +525,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -497,23 +546,11 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -522,30 +559,46 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +659,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -641,7 +694,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -825,863 +878,956 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1"/>
-    <col min="2" max="2" width="36.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1"/>
+    <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.44140625" style="1"/>
+    <col min="6" max="6" width="42.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="17">
+        <v>2.1</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:7" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G4" s="5">
         <v>43104</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G5" s="5">
         <v>43194</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G6" s="5">
         <v>43194</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G7" s="5">
         <v>43194</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="5">
         <v>43194</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="5">
         <v>43194</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="5">
         <v>43224</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G11" s="7">
         <v>43255</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G12" s="7">
         <v>43255</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7" s="18" customFormat="1" ht="13.5" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="5" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G14" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="5" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G15" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="5" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G16" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="5" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G17" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="5" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G18" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="5" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G19" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="5" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G20" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="5" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G21" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="5" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G22" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="5" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G23" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="5" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G24" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="5" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G25" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="5" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G26" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="5" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G27" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="5" t="s">
+      <c r="B28" s="8"/>
+      <c r="C28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G28" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="5" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G29" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="5" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G30" s="7">
         <v>43408</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:7" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:7" s="8" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="B32" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F32" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G32" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="B33" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E33" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F33" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G33" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+    <row r="34" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="B34" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G34" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D36" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E36" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F36" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G36" s="7">
         <v>43210</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="18" t="s">
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G37" s="7">
         <v>43210</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B37"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="B38" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="B39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="B40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
+    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
+    <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+    <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
+    <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
+    <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+    <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+    <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+    <row r="59" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:XFD12"/>
-    <mergeCell ref="A30:XFD30"/>
+    <mergeCell ref="A13:XFD13"/>
+    <mergeCell ref="A31:XFD31"/>
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D11 D13:D29 D31:D33</xm:sqref>
+          <xm:sqref>D4:D12 D14:D30 D32:D34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1690,22 +1836,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>